<commit_message>
modify  spring mapping find
</commit_message>
<xml_diff>
--- a/src/test/doc/项目进度.xlsx
+++ b/src/test/doc/项目进度.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="240">
   <si>
     <t>系统</t>
   </si>
@@ -58,9 +58,6 @@
     <t>首次查询-录入电话号码</t>
   </si>
   <si>
-    <t>开始接待</t>
-  </si>
-  <si>
     <t>选择购买商品</t>
   </si>
   <si>
@@ -251,10 +248,6 @@
   </si>
   <si>
     <t>仓库管理</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>锁定业务员显示</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -860,93 +853,105 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
+    <t>登门表</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>出单表</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>出库明细表（按照商品、礼品订单类别分别统计）</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>开发人员</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>苗文强</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>苗文强</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>夏政委</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>待定</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>订单修改管理</t>
+  </si>
+  <si>
+    <t>展厅客户对接业绩详情表</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成时间</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成情况</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>已完成</t>
+  </si>
+  <si>
+    <t>进行中</t>
+  </si>
+  <si>
+    <t>孟月</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>回购记录
+延迟</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost:8080/portal/reception/init</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>复选状态选中有问题</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>表单为空未验证</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>页面已经完成</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>锁定业务员显示</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>开始接待</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
     <t>首次登门－录入基本信息（姓名，生日，电话，地区）
 标明是否黑名单客户</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>登门表</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>出单表</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>出库明细表（按照商品、礼品订单类别分别统计）</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>A</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>开发人员</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>苗文强</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>苗文强</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>夏政委</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>待定</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>订单修改管理</t>
-  </si>
-  <si>
-    <t>展厅客户对接业绩详情表</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成时间</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>备注</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成情况</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>已完成</t>
-  </si>
-  <si>
-    <t>进行中</t>
-  </si>
-  <si>
-    <t>孟月</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>回购记录
-延迟</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://localhost:8080/portal/reception/init</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>复选状态选中有问题</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>表单为空未验证</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -2837,7 +2842,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.59765625" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2873,49 +2878,49 @@
     <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="39" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="D2" s="39" t="s">
         <v>209</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="E2" s="39" t="s">
         <v>210</v>
       </c>
-      <c r="D2" s="39" t="s">
-        <v>211</v>
-      </c>
-      <c r="E2" s="39" t="s">
-        <v>212</v>
-      </c>
       <c r="F2" s="39" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G2" s="39" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H2" s="39" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="I2" s="39" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>
       <c r="B3" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F3" s="47" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G3" s="47" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H3" s="47"/>
       <c r="I3" s="47"/>
@@ -2925,16 +2930,16 @@
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F4" s="47" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G4" s="47" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H4" s="47"/>
       <c r="I4" s="47"/>
@@ -2944,13 +2949,13 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
       <c r="D5" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F5" s="47" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G5" s="47"/>
       <c r="H5" s="47"/>
@@ -2963,16 +2968,16 @@
         <v>5</v>
       </c>
       <c r="D6" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="E6" s="40" t="s">
-        <v>99</v>
-      </c>
       <c r="F6" s="47" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H6" s="47"/>
       <c r="I6" s="47"/>
@@ -2982,16 +2987,16 @@
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E7" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F7" s="47" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G7" s="47" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H7" s="47"/>
       <c r="I7" s="47"/>
@@ -3001,13 +3006,13 @@
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
       <c r="D8" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E8" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F8" s="47" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G8" s="47"/>
       <c r="H8" s="47"/>
@@ -3017,19 +3022,19 @@
       <c r="A9" s="8"/>
       <c r="B9" s="11"/>
       <c r="C9" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F9" s="47" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G9" s="47" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H9" s="47"/>
       <c r="I9" s="47"/>
@@ -3039,16 +3044,16 @@
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F10" s="47" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G10" s="47" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H10" s="47"/>
       <c r="I10" s="47"/>
@@ -3058,13 +3063,13 @@
       <c r="B11" s="11"/>
       <c r="C11" s="12"/>
       <c r="D11" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E11" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F11" s="47" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G11" s="47"/>
       <c r="H11" s="47"/>
@@ -3074,19 +3079,19 @@
       <c r="A12" s="8"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E12" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F12" s="47" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G12" s="47" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H12" s="47"/>
       <c r="I12" s="47"/>
@@ -3096,16 +3101,16 @@
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F13" s="47" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G13" s="47" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H13" s="47"/>
       <c r="I13" s="47"/>
@@ -3118,10 +3123,10 @@
         <v>6</v>
       </c>
       <c r="E14" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F14" s="47" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G14" s="47"/>
       <c r="H14" s="47"/>
@@ -3131,16 +3136,16 @@
       <c r="A15" s="8"/>
       <c r="B15" s="11"/>
       <c r="C15" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="E15" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E15" s="40" t="s">
-        <v>102</v>
-      </c>
       <c r="F15" s="47" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G15" s="47"/>
       <c r="H15" s="47"/>
@@ -3151,13 +3156,13 @@
       <c r="B16" s="11"/>
       <c r="C16" s="17"/>
       <c r="D16" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E16" s="40" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F16" s="47" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G16" s="47"/>
       <c r="H16" s="47"/>
@@ -3168,13 +3173,13 @@
       <c r="B17" s="11"/>
       <c r="C17" s="19"/>
       <c r="D17" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E17" s="40" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F17" s="47" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G17" s="47"/>
       <c r="H17" s="47"/>
@@ -3183,7 +3188,7 @@
     <row r="18" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>8</v>
@@ -3192,17 +3197,17 @@
         <v>9</v>
       </c>
       <c r="E18" s="48" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F18" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G18" s="47" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H18" s="47"/>
       <c r="I18" s="47" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
@@ -3210,35 +3215,37 @@
       <c r="B19" s="11"/>
       <c r="C19" s="17"/>
       <c r="D19" s="18" t="s">
-        <v>216</v>
+        <v>239</v>
       </c>
       <c r="E19" s="41" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F19" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G19" s="47" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H19" s="47"/>
-      <c r="I19" s="47"/>
+      <c r="I19" s="47" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="11"/>
       <c r="C20" s="17"/>
       <c r="D20" s="15" t="s">
-        <v>72</v>
+        <v>237</v>
       </c>
       <c r="E20" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F20" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G20" s="47" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H20" s="47"/>
       <c r="I20" s="47"/>
@@ -3248,16 +3255,16 @@
       <c r="B21" s="11"/>
       <c r="C21" s="17"/>
       <c r="D21" s="15" t="s">
-        <v>10</v>
+        <v>238</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F21" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G21" s="47" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H21" s="47"/>
       <c r="I21" s="47"/>
@@ -3267,20 +3274,20 @@
       <c r="B22" s="11"/>
       <c r="C22" s="17"/>
       <c r="D22" s="18" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E22" s="43" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F22" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G22" s="47" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H22" s="47"/>
       <c r="I22" s="47" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -3288,13 +3295,13 @@
       <c r="B23" s="11"/>
       <c r="C23" s="17"/>
       <c r="D23" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E23" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F23" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G23" s="47"/>
       <c r="H23" s="47"/>
@@ -3305,13 +3312,13 @@
       <c r="B24" s="11"/>
       <c r="C24" s="17"/>
       <c r="D24" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E24" s="40" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F24" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G24" s="47"/>
       <c r="H24" s="47"/>
@@ -3322,13 +3329,13 @@
       <c r="B25" s="11"/>
       <c r="C25" s="17"/>
       <c r="D25" s="15" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E25" s="40" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F25" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G25" s="47"/>
       <c r="H25" s="47"/>
@@ -3339,13 +3346,13 @@
       <c r="B26" s="11"/>
       <c r="C26" s="17"/>
       <c r="D26" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E26" s="40" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F26" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G26" s="47"/>
       <c r="H26" s="47"/>
@@ -3355,16 +3362,16 @@
       <c r="A27" s="8"/>
       <c r="B27" s="11"/>
       <c r="C27" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="D27" s="15" t="s">
-        <v>106</v>
-      </c>
       <c r="E27" s="40" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F27" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G27" s="47"/>
       <c r="H27" s="47"/>
@@ -3375,13 +3382,13 @@
       <c r="B28" s="11"/>
       <c r="C28" s="17"/>
       <c r="D28" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E28" s="40" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F28" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G28" s="47"/>
       <c r="H28" s="47"/>
@@ -3392,13 +3399,13 @@
       <c r="B29" s="11"/>
       <c r="C29" s="17"/>
       <c r="D29" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E29" s="40" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F29" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G29" s="47"/>
       <c r="H29" s="47"/>
@@ -3409,13 +3416,13 @@
       <c r="B30" s="11"/>
       <c r="C30" s="19"/>
       <c r="D30" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E30" s="40" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F30" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G30" s="47"/>
       <c r="H30" s="47"/>
@@ -3425,23 +3432,23 @@
       <c r="A31" s="8"/>
       <c r="B31" s="11"/>
       <c r="C31" s="20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E31" s="40" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F31" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G31" s="47" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H31" s="47"/>
       <c r="I31" s="56" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3449,36 +3456,36 @@
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
       <c r="D32" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E32" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F32" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G32" s="47" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H32" s="47"/>
       <c r="I32" s="47" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="11"/>
       <c r="C33" s="23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E33" s="40" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F33" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G33" s="47"/>
       <c r="H33" s="47"/>
@@ -3489,13 +3496,13 @@
       <c r="B34" s="11"/>
       <c r="C34" s="17"/>
       <c r="D34" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E34" s="40" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F34" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G34" s="47"/>
       <c r="H34" s="47"/>
@@ -3506,13 +3513,13 @@
       <c r="B35" s="11"/>
       <c r="C35" s="19"/>
       <c r="D35" s="15" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E35" s="40" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F35" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G35" s="47"/>
       <c r="H35" s="47"/>
@@ -3525,13 +3532,13 @@
         <v>7</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E36" s="42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F36" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G36" s="47"/>
       <c r="H36" s="47"/>
@@ -3542,13 +3549,13 @@
       <c r="B37" s="11"/>
       <c r="C37" s="17"/>
       <c r="D37" s="18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E37" s="42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F37" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G37" s="47"/>
       <c r="H37" s="47"/>
@@ -3559,13 +3566,13 @@
       <c r="B38" s="11"/>
       <c r="C38" s="17"/>
       <c r="D38" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E38" s="42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F38" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G38" s="47"/>
       <c r="H38" s="47"/>
@@ -3576,13 +3583,13 @@
       <c r="B39" s="11"/>
       <c r="C39" s="17"/>
       <c r="D39" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E39" s="42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F39" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G39" s="47"/>
       <c r="H39" s="47"/>
@@ -3593,13 +3600,13 @@
       <c r="B40" s="11"/>
       <c r="C40" s="17"/>
       <c r="D40" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E40" s="42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F40" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G40" s="47"/>
       <c r="H40" s="47"/>
@@ -3609,16 +3616,16 @@
       <c r="A41" s="8"/>
       <c r="B41" s="11"/>
       <c r="C41" s="23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E41" s="42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F41" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G41" s="47"/>
       <c r="H41" s="47"/>
@@ -3629,13 +3636,13 @@
       <c r="B42" s="11"/>
       <c r="C42" s="17"/>
       <c r="D42" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E42" s="42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F42" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G42" s="47"/>
       <c r="H42" s="47"/>
@@ -3645,16 +3652,16 @@
       <c r="A43" s="8"/>
       <c r="B43" s="25"/>
       <c r="C43" s="23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E43" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F43" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G43" s="47"/>
       <c r="H43" s="47"/>
@@ -3665,13 +3672,13 @@
       <c r="B44" s="25"/>
       <c r="C44" s="24"/>
       <c r="D44" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E44" s="42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F44" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G44" s="47"/>
       <c r="H44" s="47"/>
@@ -3682,13 +3689,13 @@
       <c r="B45" s="25"/>
       <c r="C45" s="17"/>
       <c r="D45" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E45" s="42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F45" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G45" s="47"/>
       <c r="H45" s="47"/>
@@ -3699,13 +3706,13 @@
       <c r="B46" s="25"/>
       <c r="C46" s="17"/>
       <c r="D46" s="15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E46" s="42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F46" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G46" s="47"/>
       <c r="H46" s="47"/>
@@ -3716,11 +3723,11 @@
       <c r="B47" s="25"/>
       <c r="C47" s="19"/>
       <c r="D47" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E47" s="42"/>
       <c r="F47" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G47" s="47"/>
       <c r="H47" s="47"/>
@@ -3729,19 +3736,19 @@
     <row r="48" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="8"/>
       <c r="B48" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E48" s="40" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F48" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G48" s="47"/>
       <c r="H48" s="47"/>
@@ -3752,13 +3759,13 @@
       <c r="B49" s="11"/>
       <c r="C49" s="19"/>
       <c r="D49" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E49" s="40" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F49" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G49" s="47"/>
       <c r="H49" s="47"/>
@@ -3768,16 +3775,16 @@
       <c r="A50" s="8"/>
       <c r="B50" s="11"/>
       <c r="C50" s="23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E50" s="40" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F50" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G50" s="47"/>
       <c r="H50" s="47"/>
@@ -3788,13 +3795,13 @@
       <c r="B51" s="11"/>
       <c r="C51" s="19"/>
       <c r="D51" s="15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E51" s="40" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F51" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G51" s="47"/>
       <c r="H51" s="47"/>
@@ -3804,16 +3811,16 @@
       <c r="A52" s="8"/>
       <c r="B52" s="11"/>
       <c r="C52" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E52" s="42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F52" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G52" s="47"/>
       <c r="H52" s="47"/>
@@ -3824,13 +3831,13 @@
       <c r="B53" s="11"/>
       <c r="C53" s="11"/>
       <c r="D53" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E53" s="42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F53" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G53" s="47"/>
       <c r="H53" s="47"/>
@@ -3841,13 +3848,13 @@
       <c r="B54" s="11"/>
       <c r="C54" s="11"/>
       <c r="D54" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E54" s="42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F54" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G54" s="47"/>
       <c r="H54" s="47"/>
@@ -3857,16 +3864,16 @@
       <c r="A55" s="8"/>
       <c r="B55" s="25"/>
       <c r="C55" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D55" s="15" t="s">
-        <v>14</v>
-      </c>
       <c r="E55" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F55" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G55" s="47"/>
       <c r="H55" s="47"/>
@@ -3877,13 +3884,13 @@
       <c r="B56" s="25"/>
       <c r="C56" s="17"/>
       <c r="D56" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E56" s="40" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F56" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G56" s="47"/>
       <c r="H56" s="47"/>
@@ -3894,13 +3901,13 @@
       <c r="B57" s="25"/>
       <c r="C57" s="17"/>
       <c r="D57" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E57" s="40" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F57" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G57" s="47"/>
       <c r="H57" s="47"/>
@@ -3911,13 +3918,13 @@
       <c r="B58" s="25"/>
       <c r="C58" s="17"/>
       <c r="D58" s="15" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E58" s="40" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F58" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G58" s="47"/>
       <c r="H58" s="47"/>
@@ -3928,13 +3935,13 @@
       <c r="B59" s="25"/>
       <c r="C59" s="17"/>
       <c r="D59" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E59" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F59" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G59" s="47"/>
       <c r="H59" s="47"/>
@@ -3945,13 +3952,13 @@
       <c r="B60" s="25"/>
       <c r="C60" s="17"/>
       <c r="D60" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E60" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F60" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G60" s="47"/>
       <c r="H60" s="47"/>
@@ -3962,13 +3969,13 @@
       <c r="B61" s="25"/>
       <c r="C61" s="17"/>
       <c r="D61" s="15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E61" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F61" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G61" s="47"/>
       <c r="H61" s="47"/>
@@ -3979,13 +3986,13 @@
       <c r="B62" s="25"/>
       <c r="C62" s="19"/>
       <c r="D62" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E62" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F62" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G62" s="47"/>
       <c r="H62" s="47"/>
@@ -3995,16 +4002,16 @@
       <c r="A63" s="8"/>
       <c r="B63" s="11"/>
       <c r="C63" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E63" s="42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F63" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G63" s="47"/>
       <c r="H63" s="47"/>
@@ -4015,13 +4022,13 @@
       <c r="B64" s="11"/>
       <c r="C64" s="20"/>
       <c r="D64" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E64" s="42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F64" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G64" s="47"/>
       <c r="H64" s="47"/>
@@ -4032,13 +4039,13 @@
       <c r="B65" s="11"/>
       <c r="C65" s="20"/>
       <c r="D65" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E65" s="42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F65" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G65" s="47"/>
       <c r="H65" s="47"/>
@@ -4049,13 +4056,13 @@
       <c r="B66" s="11"/>
       <c r="C66" s="20"/>
       <c r="D66" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E66" s="42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F66" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G66" s="47"/>
       <c r="H66" s="47"/>
@@ -4066,13 +4073,13 @@
       <c r="B67" s="11"/>
       <c r="C67" s="20"/>
       <c r="D67" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E67" s="42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F67" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G67" s="47"/>
       <c r="H67" s="47"/>
@@ -4083,13 +4090,13 @@
       <c r="B68" s="11"/>
       <c r="C68" s="20"/>
       <c r="D68" s="10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E68" s="42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F68" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G68" s="47"/>
       <c r="H68" s="47"/>
@@ -4100,13 +4107,13 @@
       <c r="B69" s="11"/>
       <c r="C69" s="20"/>
       <c r="D69" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E69" s="42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F69" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G69" s="47"/>
       <c r="H69" s="47"/>
@@ -4116,16 +4123,16 @@
       <c r="A70" s="8"/>
       <c r="B70" s="11"/>
       <c r="C70" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E70" s="42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F70" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G70" s="47"/>
       <c r="H70" s="47"/>
@@ -4136,13 +4143,13 @@
       <c r="B71" s="11"/>
       <c r="C71" s="11"/>
       <c r="D71" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E71" s="42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F71" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G71" s="47"/>
       <c r="H71" s="47"/>
@@ -4153,13 +4160,13 @@
       <c r="B72" s="11"/>
       <c r="C72" s="11"/>
       <c r="D72" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E72" s="42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F72" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G72" s="47"/>
       <c r="H72" s="47"/>
@@ -4170,13 +4177,13 @@
       <c r="B73" s="11"/>
       <c r="C73" s="11"/>
       <c r="D73" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E73" s="42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F73" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G73" s="47"/>
       <c r="H73" s="47"/>
@@ -4187,13 +4194,13 @@
       <c r="B74" s="11"/>
       <c r="C74" s="11"/>
       <c r="D74" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E74" s="42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F74" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G74" s="47"/>
       <c r="H74" s="47"/>
@@ -4204,13 +4211,13 @@
       <c r="B75" s="11"/>
       <c r="C75" s="11"/>
       <c r="D75" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E75" s="42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F75" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G75" s="47"/>
       <c r="H75" s="47"/>
@@ -4221,13 +4228,13 @@
       <c r="B76" s="11"/>
       <c r="C76" s="11"/>
       <c r="D76" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E76" s="42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F76" s="47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G76" s="47"/>
       <c r="H76" s="47"/>
@@ -4236,22 +4243,22 @@
     <row r="77" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4"/>
       <c r="B77" s="23" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C77" s="33" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D77" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E77" s="48" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F77" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G77" s="47" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H77" s="47"/>
       <c r="I77" s="47"/>
@@ -4261,16 +4268,16 @@
       <c r="B78" s="17"/>
       <c r="C78" s="29"/>
       <c r="D78" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E78" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F78" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G78" s="47" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H78" s="47"/>
       <c r="I78" s="47"/>
@@ -4280,16 +4287,16 @@
       <c r="B79" s="17"/>
       <c r="C79" s="29"/>
       <c r="D79" s="15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E79" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F79" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G79" s="47" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H79" s="47"/>
       <c r="I79" s="47"/>
@@ -4299,16 +4306,16 @@
       <c r="B80" s="17"/>
       <c r="C80" s="29"/>
       <c r="D80" s="15" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E80" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F80" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G80" s="47" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H80" s="47"/>
       <c r="I80" s="47"/>
@@ -4318,16 +4325,16 @@
       <c r="B81" s="17"/>
       <c r="C81" s="29"/>
       <c r="D81" s="15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E81" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F81" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G81" s="47" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H81" s="47"/>
       <c r="I81" s="47"/>
@@ -4337,16 +4344,16 @@
       <c r="B82" s="17"/>
       <c r="C82" s="29"/>
       <c r="D82" s="15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E82" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F82" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G82" s="47" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H82" s="47"/>
       <c r="I82" s="47"/>
@@ -4355,16 +4362,16 @@
       <c r="A83" s="4"/>
       <c r="B83" s="50"/>
       <c r="C83" s="49" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D83" s="15" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E83" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F83" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G83" s="47"/>
       <c r="H83" s="47"/>
@@ -4374,16 +4381,16 @@
       <c r="A84" s="4"/>
       <c r="B84" s="17"/>
       <c r="C84" s="29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D84" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E84" s="42" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F84" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G84" s="47"/>
       <c r="H84" s="47"/>
@@ -4394,13 +4401,13 @@
       <c r="B85" s="17"/>
       <c r="C85" s="29"/>
       <c r="D85" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E85" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F85" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G85" s="47"/>
       <c r="H85" s="47"/>
@@ -4411,13 +4418,13 @@
       <c r="B86" s="17"/>
       <c r="C86" s="29"/>
       <c r="D86" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E86" s="42" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F86" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G86" s="47"/>
       <c r="H86" s="47"/>
@@ -4428,13 +4435,13 @@
       <c r="B87" s="17"/>
       <c r="C87" s="29"/>
       <c r="D87" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E87" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F87" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G87" s="47"/>
       <c r="H87" s="47"/>
@@ -4445,13 +4452,13 @@
       <c r="B88" s="17"/>
       <c r="C88" s="29"/>
       <c r="D88" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E88" s="42" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F88" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G88" s="47"/>
       <c r="H88" s="47"/>
@@ -4462,13 +4469,13 @@
       <c r="B89" s="17"/>
       <c r="C89" s="29"/>
       <c r="D89" s="15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E89" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F89" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G89" s="47"/>
       <c r="H89" s="47"/>
@@ -4478,16 +4485,16 @@
       <c r="A90" s="4"/>
       <c r="B90" s="17"/>
       <c r="C90" s="28" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D90" s="15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E90" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F90" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G90" s="47"/>
       <c r="H90" s="47"/>
@@ -4498,13 +4505,13 @@
       <c r="B91" s="17"/>
       <c r="C91" s="30"/>
       <c r="D91" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E91" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F91" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G91" s="47"/>
       <c r="H91" s="47"/>
@@ -4514,16 +4521,16 @@
       <c r="A92" s="4"/>
       <c r="B92" s="17"/>
       <c r="C92" s="28" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D92" s="15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E92" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F92" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G92" s="47"/>
       <c r="H92" s="47"/>
@@ -4534,13 +4541,13 @@
       <c r="B93" s="17"/>
       <c r="C93" s="29"/>
       <c r="D93" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E93" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F93" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G93" s="47"/>
       <c r="H93" s="47"/>
@@ -4550,16 +4557,16 @@
       <c r="A94" s="4"/>
       <c r="B94" s="17"/>
       <c r="C94" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D94" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E94" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F94" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G94" s="47"/>
       <c r="H94" s="47"/>
@@ -4569,16 +4576,16 @@
       <c r="A95" s="4"/>
       <c r="B95" s="17"/>
       <c r="C95" s="29" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D95" s="15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E95" s="42" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F95" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G95" s="47"/>
       <c r="H95" s="47"/>
@@ -4589,13 +4596,13 @@
       <c r="B96" s="17"/>
       <c r="C96" s="29"/>
       <c r="D96" s="15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E96" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F96" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G96" s="47"/>
       <c r="H96" s="47"/>
@@ -4606,13 +4613,13 @@
       <c r="B97" s="17"/>
       <c r="C97" s="29"/>
       <c r="D97" s="15" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E97" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F97" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G97" s="47"/>
       <c r="H97" s="47"/>
@@ -4623,13 +4630,13 @@
       <c r="B98" s="17"/>
       <c r="C98" s="30"/>
       <c r="D98" s="15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E98" s="42" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F98" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G98" s="47"/>
       <c r="H98" s="47"/>
@@ -4639,16 +4646,16 @@
       <c r="A99" s="4"/>
       <c r="B99" s="17"/>
       <c r="C99" s="28" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D99" s="15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E99" s="42" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F99" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G99" s="47"/>
       <c r="H99" s="47"/>
@@ -4659,13 +4666,13 @@
       <c r="B100" s="17"/>
       <c r="C100" s="29"/>
       <c r="D100" s="15" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E100" s="42" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F100" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G100" s="47"/>
       <c r="H100" s="47"/>
@@ -4676,13 +4683,13 @@
       <c r="B101" s="17"/>
       <c r="C101" s="30"/>
       <c r="D101" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E101" s="42" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F101" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G101" s="47"/>
       <c r="H101" s="47"/>
@@ -4692,16 +4699,16 @@
       <c r="A102" s="4"/>
       <c r="B102" s="17"/>
       <c r="C102" s="28" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D102" s="15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E102" s="42" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F102" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G102" s="47"/>
       <c r="H102" s="47"/>
@@ -4712,13 +4719,13 @@
       <c r="B103" s="17"/>
       <c r="C103" s="30"/>
       <c r="D103" s="15" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E103" s="42" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F103" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G103" s="47"/>
       <c r="H103" s="47"/>
@@ -4727,19 +4734,19 @@
     <row r="104" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="4"/>
       <c r="B104" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C104" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D104" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D104" s="15" t="s">
-        <v>16</v>
-      </c>
       <c r="E104" s="48" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F104" s="47" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G104" s="47"/>
       <c r="H104" s="47"/>
@@ -4750,13 +4757,13 @@
       <c r="B105" s="17"/>
       <c r="C105" s="35"/>
       <c r="D105" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E105" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F105" s="47" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G105" s="47"/>
       <c r="H105" s="47"/>
@@ -4767,13 +4774,13 @@
       <c r="B106" s="17"/>
       <c r="C106" s="30"/>
       <c r="D106" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E106" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F106" s="47" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G106" s="47"/>
       <c r="H106" s="47"/>
@@ -4783,16 +4790,16 @@
       <c r="A107" s="4"/>
       <c r="B107" s="17"/>
       <c r="C107" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D107" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D107" s="10" t="s">
-        <v>20</v>
-      </c>
       <c r="E107" s="42" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F107" s="47" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G107" s="47"/>
       <c r="H107" s="47"/>
@@ -4802,16 +4809,16 @@
       <c r="A108" s="4"/>
       <c r="B108" s="17"/>
       <c r="C108" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D108" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D108" s="10" t="s">
-        <v>22</v>
-      </c>
       <c r="E108" s="42" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F108" s="47" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G108" s="47"/>
       <c r="H108" s="47"/>
@@ -4821,16 +4828,16 @@
       <c r="A109" s="4"/>
       <c r="B109" s="32"/>
       <c r="C109" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D109" s="10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E109" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F109" s="47" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G109" s="47"/>
       <c r="H109" s="47"/>
@@ -4839,19 +4846,19 @@
     <row r="110" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="8"/>
       <c r="B110" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C110" s="52" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D110" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E110" s="48" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F110" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G110" s="47"/>
       <c r="H110" s="47"/>
@@ -4862,13 +4869,13 @@
       <c r="B111" s="11"/>
       <c r="C111" s="53"/>
       <c r="D111" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E111" s="42" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F111" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G111" s="47"/>
       <c r="H111" s="47"/>
@@ -4879,13 +4886,13 @@
       <c r="B112" s="11"/>
       <c r="C112" s="53"/>
       <c r="D112" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E112" s="42" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F112" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G112" s="47"/>
       <c r="H112" s="47"/>
@@ -4895,13 +4902,13 @@
       <c r="A113" s="8"/>
       <c r="B113" s="11"/>
       <c r="D113" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E113" s="42" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F113" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G113" s="47"/>
       <c r="H113" s="47"/>
@@ -4911,13 +4918,13 @@
       <c r="A114" s="8"/>
       <c r="B114" s="11"/>
       <c r="D114" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E114" s="42" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F114" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G114" s="47"/>
       <c r="H114" s="47"/>
@@ -4927,13 +4934,13 @@
       <c r="A115" s="8"/>
       <c r="B115" s="11"/>
       <c r="D115" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E115" s="42" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F115" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G115" s="47"/>
       <c r="H115" s="47"/>
@@ -4943,13 +4950,13 @@
       <c r="A116" s="8"/>
       <c r="B116" s="11"/>
       <c r="D116" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E116" s="42" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F116" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G116" s="47"/>
       <c r="H116" s="47"/>
@@ -4959,13 +4966,13 @@
       <c r="A117" s="8"/>
       <c r="B117" s="11"/>
       <c r="D117" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E117" s="42" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F117" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G117" s="47"/>
       <c r="H117" s="47"/>
@@ -4974,22 +4981,22 @@
     <row r="118" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="4"/>
       <c r="B118" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C118" s="54" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D118" s="27" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E118" s="40" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F118" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G118" s="47" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H118" s="51">
         <v>42651</v>
@@ -5001,16 +5008,16 @@
       <c r="B119" s="31"/>
       <c r="C119" s="55"/>
       <c r="D119" s="27" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E119" s="40" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F119" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G119" s="47" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H119" s="51">
         <v>42651</v>
@@ -5022,16 +5029,16 @@
       <c r="B120" s="31"/>
       <c r="C120" s="55"/>
       <c r="D120" s="27" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E120" s="40" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F120" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G120" s="47" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H120" s="47"/>
       <c r="I120" s="47"/>
@@ -5041,16 +5048,16 @@
       <c r="B121" s="31"/>
       <c r="C121" s="55"/>
       <c r="D121" s="27" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E121" s="40" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F121" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G121" s="47" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H121" s="51">
         <v>42655</v>
@@ -5062,16 +5069,16 @@
       <c r="B122" s="31"/>
       <c r="C122" s="55"/>
       <c r="D122" s="27" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E122" s="40" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F122" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G122" s="47" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H122" s="51">
         <v>42655</v>
@@ -5083,16 +5090,16 @@
       <c r="B123" s="31"/>
       <c r="C123" s="55"/>
       <c r="D123" s="27" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E123" s="40" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F123" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G123" s="47" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H123" s="51">
         <v>42655</v>
@@ -5104,16 +5111,16 @@
       <c r="B124" s="31"/>
       <c r="C124" s="55"/>
       <c r="D124" s="27" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E124" s="40" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F124" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G124" s="47" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H124" s="51">
         <v>42656</v>
@@ -5125,16 +5132,16 @@
       <c r="B125" s="31"/>
       <c r="C125" s="55"/>
       <c r="D125" s="27" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E125" s="40" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F125" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G125" s="47" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H125" s="51">
         <v>42657</v>
@@ -5146,16 +5153,16 @@
       <c r="B126" s="31"/>
       <c r="C126" s="55"/>
       <c r="D126" s="27" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E126" s="40" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F126" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G126" s="47" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H126" s="51">
         <v>42661</v>
@@ -5167,16 +5174,16 @@
       <c r="B127" s="31"/>
       <c r="C127" s="55"/>
       <c r="D127" s="27" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E127" s="40" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F127" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G127" s="47" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H127" s="51">
         <v>42661</v>
@@ -5188,16 +5195,16 @@
       <c r="B128" s="31"/>
       <c r="C128" s="45"/>
       <c r="D128" s="27" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E128" s="40" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F128" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G128" s="47" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H128" s="51">
         <v>42664</v>
@@ -5209,16 +5216,16 @@
       <c r="B129" s="31"/>
       <c r="C129" s="29"/>
       <c r="D129" s="27" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E129" s="40" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F129" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G129" s="47" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H129" s="51">
         <v>42667</v>
@@ -5229,16 +5236,16 @@
       <c r="A130" s="4"/>
       <c r="B130" s="31"/>
       <c r="C130" s="28" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D130" s="27" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E130" s="40" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F130" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G130" s="47"/>
       <c r="H130" s="47"/>
@@ -5249,13 +5256,13 @@
       <c r="B131" s="32"/>
       <c r="C131" s="30"/>
       <c r="D131" s="27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E131" s="40" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F131" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G131" s="47"/>
       <c r="H131" s="47"/>
@@ -5264,19 +5271,19 @@
     <row r="132" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="8"/>
       <c r="B132" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C132" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D132" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D132" s="10" t="s">
-        <v>33</v>
-      </c>
       <c r="E132" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F132" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G132" s="47"/>
       <c r="H132" s="47"/>
@@ -5287,13 +5294,13 @@
       <c r="B133" s="20"/>
       <c r="C133" s="20"/>
       <c r="D133" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E133" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F133" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G133" s="47"/>
       <c r="H133" s="47"/>
@@ -5304,13 +5311,13 @@
       <c r="B134" s="11"/>
       <c r="C134" s="11"/>
       <c r="D134" s="10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E134" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F134" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G134" s="47"/>
       <c r="H134" s="47"/>
@@ -5321,13 +5328,13 @@
       <c r="B135" s="11"/>
       <c r="C135" s="11"/>
       <c r="D135" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E135" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F135" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G135" s="47"/>
       <c r="H135" s="47"/>
@@ -5338,13 +5345,13 @@
       <c r="B136" s="11"/>
       <c r="C136" s="12"/>
       <c r="D136" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E136" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F136" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G136" s="47"/>
       <c r="H136" s="47"/>
@@ -5354,16 +5361,16 @@
       <c r="A137" s="8"/>
       <c r="B137" s="11"/>
       <c r="C137" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D137" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D137" s="10" t="s">
-        <v>37</v>
-      </c>
       <c r="E137" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F137" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G137" s="47"/>
       <c r="H137" s="47"/>
@@ -5374,13 +5381,13 @@
       <c r="B138" s="11"/>
       <c r="C138" s="11"/>
       <c r="D138" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E138" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F138" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G138" s="47"/>
       <c r="H138" s="47"/>
@@ -5391,13 +5398,13 @@
       <c r="B139" s="11"/>
       <c r="C139" s="12"/>
       <c r="D139" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E139" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F139" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G139" s="47"/>
       <c r="H139" s="47"/>
@@ -5407,16 +5414,16 @@
       <c r="A140" s="8"/>
       <c r="B140" s="11"/>
       <c r="C140" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D140" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D140" s="10" t="s">
-        <v>41</v>
-      </c>
       <c r="E140" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F140" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G140" s="47"/>
       <c r="H140" s="47"/>
@@ -5427,13 +5434,13 @@
       <c r="B141" s="11"/>
       <c r="C141" s="11"/>
       <c r="D141" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E141" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F141" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G141" s="47"/>
       <c r="H141" s="47"/>
@@ -5444,13 +5451,13 @@
       <c r="B142" s="11"/>
       <c r="C142" s="12"/>
       <c r="D142" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E142" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F142" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G142" s="47"/>
       <c r="H142" s="47"/>
@@ -5460,16 +5467,16 @@
       <c r="A143" s="8"/>
       <c r="B143" s="11"/>
       <c r="C143" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D143" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D143" s="10" t="s">
-        <v>45</v>
-      </c>
       <c r="E143" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F143" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G143" s="47"/>
       <c r="H143" s="47"/>
@@ -5480,13 +5487,13 @@
       <c r="B144" s="11"/>
       <c r="C144" s="11"/>
       <c r="D144" s="10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E144" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F144" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G144" s="47"/>
       <c r="H144" s="47"/>
@@ -5497,13 +5504,13 @@
       <c r="B145" s="11"/>
       <c r="C145" s="12"/>
       <c r="D145" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E145" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F145" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G145" s="47"/>
       <c r="H145" s="47"/>
@@ -5513,16 +5520,16 @@
       <c r="A146" s="8"/>
       <c r="B146" s="11"/>
       <c r="C146" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D146" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D146" s="10" t="s">
-        <v>48</v>
-      </c>
       <c r="E146" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F146" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G146" s="47"/>
       <c r="H146" s="47"/>
@@ -5533,13 +5540,13 @@
       <c r="B147" s="11"/>
       <c r="C147" s="12"/>
       <c r="D147" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E147" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F147" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G147" s="47"/>
       <c r="H147" s="47"/>
@@ -5549,16 +5556,16 @@
       <c r="A148" s="8"/>
       <c r="B148" s="11"/>
       <c r="C148" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D148" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D148" s="10" t="s">
-        <v>51</v>
-      </c>
       <c r="E148" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F148" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G148" s="47"/>
       <c r="H148" s="47"/>
@@ -5569,13 +5576,13 @@
       <c r="B149" s="11"/>
       <c r="C149" s="11"/>
       <c r="D149" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E149" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F149" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G149" s="47"/>
       <c r="H149" s="47"/>
@@ -5586,13 +5593,13 @@
       <c r="B150" s="11"/>
       <c r="C150" s="11"/>
       <c r="D150" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E150" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F150" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G150" s="47"/>
       <c r="H150" s="47"/>
@@ -5603,13 +5610,13 @@
       <c r="B151" s="11"/>
       <c r="C151" s="12"/>
       <c r="D151" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E151" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F151" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G151" s="47"/>
       <c r="H151" s="47"/>
@@ -5619,16 +5626,16 @@
       <c r="A152" s="8"/>
       <c r="B152" s="11"/>
       <c r="C152" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D152" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D152" s="10" t="s">
-        <v>56</v>
-      </c>
       <c r="E152" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F152" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G152" s="47"/>
       <c r="H152" s="47"/>
@@ -5638,16 +5645,16 @@
       <c r="A153" s="8"/>
       <c r="B153" s="11"/>
       <c r="C153" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D153" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D153" s="10" t="s">
-        <v>58</v>
-      </c>
       <c r="E153" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F153" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G153" s="47"/>
       <c r="H153" s="47"/>
@@ -5658,13 +5665,13 @@
       <c r="B154" s="11"/>
       <c r="C154" s="12"/>
       <c r="D154" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E154" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F154" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G154" s="47"/>
       <c r="H154" s="47"/>
@@ -5674,16 +5681,16 @@
       <c r="A155" s="8"/>
       <c r="B155" s="37"/>
       <c r="C155" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D155" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D155" s="10" t="s">
-        <v>61</v>
-      </c>
       <c r="E155" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F155" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G155" s="47"/>
       <c r="H155" s="47"/>

</xml_diff>